<commit_message>
began schematic rev 3.0
</commit_message>
<xml_diff>
--- a/rough BoM.xlsx
+++ b/rough BoM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Secction</t>
   </si>
@@ -133,6 +133,24 @@
   </si>
   <si>
     <t>https://jlcpcb.com/partdetail/Hynetek-HUSB237_AA001DN06R/C22373734</t>
+  </si>
+  <si>
+    <t>analog switch</t>
+  </si>
+  <si>
+    <t>SN74LVC1G3157DCKR</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/TexasInstruments-SN74LVC1G3157DCKR/C38663</t>
+  </si>
+  <si>
+    <t>On/Off switch</t>
+  </si>
+  <si>
+    <t>SK22D15L5</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/XkbConnection-SK22D15L5/C2884795</t>
   </si>
 </sst>
 </file>
@@ -487,14 +505,14 @@
   <dimension ref="A2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -626,7 +644,7 @@
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="L8" t="s">
@@ -651,6 +669,26 @@
       </c>
       <c r="F9" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>5.1299999999999998E-2</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -661,7 +699,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="3">
         <f>SUM(D5:E13)</f>
-        <v>13.8672</v>
+        <v>16.918500000000002</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -703,6 +741,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19">
+        <v>0.31</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>17</v>
@@ -711,7 +769,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3">
         <f>SUM(D19:E24)</f>
-        <v>0</v>
+        <v>3.31</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -724,7 +782,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2">
         <f>D25+D14</f>
-        <v>13.8672</v>
+        <v>20.2285</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -747,7 +805,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2">
         <f>D28-D27</f>
-        <v>42.632800000000003</v>
+        <v>36.271500000000003</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -755,8 +813,9 @@
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
     <hyperlink ref="F6" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>